<commit_message>
full playable set basically implemented with complete deck, card removal from board, and filling in new random cards from deck.
</commit_message>
<xml_diff>
--- a/pokesetChecklist.xlsx
+++ b/pokesetChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Camnitz\Desktop\codeTemple\capstoneProjects\pokeSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6697CED0-006C-40CA-8C7A-CBC3929F0F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B0E7E6-C280-455B-9351-ADDA56681378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17895" yWindow="1215" windowWidth="11340" windowHeight="13275" xr2:uid="{681FEDFD-4A6F-4A19-B247-930FBB9293F8}"/>
+    <workbookView xWindow="16065" yWindow="1335" windowWidth="11340" windowHeight="13275" xr2:uid="{681FEDFD-4A6F-4A19-B247-930FBB9293F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>App Checklist</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>remove successful set cards</t>
+  </si>
+  <si>
+    <t>add user feedback for clicks, successful set, total sets found</t>
   </si>
 </sst>
 </file>
@@ -509,13 +512,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430B6BA9-5F94-4D0E-B360-B27B7E705A98}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,80 +640,86 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>